<commit_message>
add fret markers to side of fretboard
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Orion_Programs\!Source_Controlled\Avera-G60-Guitar-Design\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4E9E4B-B32E-4166-A3AC-2ABFC3089953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EFB1CE-B65A-4CE1-A17E-16DF48CF962F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{C87BB195-3105-479C-84A5-3F121CF8484B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="2" r:id="rId1"/>
-    <sheet name="Total" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
   <si>
     <t>Part</t>
   </si>
@@ -130,9 +129,6 @@
     <t>Fret Markers</t>
   </si>
   <si>
-    <t>Stainless Steel barstock</t>
-  </si>
-  <si>
     <t>Neck Reinforcement</t>
   </si>
   <si>
@@ -208,9 +204,6 @@
     <t xml:space="preserve">https://www.digikey.ca/en/products/detail/c-k/JS202011CQN/1640097?so=83209932&amp;content=productdetail_CA </t>
   </si>
   <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
     <t>Cost ($CAD)</t>
   </si>
   <si>
@@ -257,13 +250,34 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.ca/en/products/detail/bourns-inc/PDB183-GTR02-504A2/3780731?so=83209932&amp;content=productdetail_CA </t>
+  </si>
+  <si>
+    <t>Stainless Steel barstock 2.5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.ca/uxcell-2-5mm-300mm-Stainless-Steel/dp/B082ZP51H5/ref=sr_1_8?crid=O8FOT18VKVES&amp;keywords=stainless+steel+bar+stock+2.5mm&amp;qid=1699750011&amp;sprefix=stainless+steel+bar+stock+2+5mm%2Caps%2C96&amp;sr=8-8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/switchcraft-inc/11/109515 </t>
+  </si>
+  <si>
+    <t>SC1085-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.metalsupermarkets.com/metals/aluminum/ </t>
+  </si>
+  <si>
+    <t>2K Clear</t>
+  </si>
+  <si>
+    <t>Total Cost ($CAD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +298,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -400,18 +421,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -731,7 +753,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -746,25 +768,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2"/>
@@ -774,12 +796,12 @@
         <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
         <v>15.02</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -788,8 +810,8 @@
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>37</v>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -797,12 +819,12 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -811,8 +833,8 @@
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>38</v>
+      <c r="G3" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -820,12 +842,12 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>132</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -834,8 +856,8 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>39</v>
+      <c r="G4" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -843,12 +865,12 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>236</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -857,8 +879,8 @@
       <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>40</v>
+      <c r="G5" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
@@ -866,31 +888,39 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="7">
+        <v>5.77</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>45.52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>75</v>
+        <v>40</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -898,19 +928,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>18.62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>76</v>
+        <v>53</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
@@ -918,19 +948,19 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>4.28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
@@ -938,17 +968,22 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="7">
+        <v>10</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -956,19 +991,19 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>4.2699999999999996</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
@@ -976,12 +1011,12 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -990,8 +1025,8 @@
       <c r="F12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>56</v>
+      <c r="G12" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -999,22 +1034,22 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>106.4</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>74</v>
+      <c r="G13" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
@@ -1022,12 +1057,12 @@
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <v>104</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1036,8 +1071,8 @@
       <c r="F14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>64</v>
+      <c r="G14" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -1045,19 +1080,19 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>22.7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="8" t="s">
         <v>71</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
@@ -1065,19 +1100,19 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <v>38</v>
       </c>
       <c r="E16" s="1">
         <v>14010201</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>72</v>
+      <c r="G16" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -1085,14 +1120,14 @@
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="D17" s="7"/>
       <c r="E17" s="1">
         <v>6105</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>68</v>
+      <c r="G17" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -1100,90 +1135,106 @@
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="10"/>
+        <v>52</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>13.49</v>
+      </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>75</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="7"/>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="F20" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="F20" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="F22" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D23" s="10"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D24" s="10"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D25" s="10"/>
+      <c r="D25" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D26" s="10"/>
+      <c r="D26" s="7">
+        <f>SUM(D2:D23)</f>
+        <v>920.06999999999994</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D27" s="10"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D28" s="10"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D29" s="10"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D30" s="10"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D31" s="10"/>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D32" s="10"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D33" s="10"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D34" s="10"/>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D35" s="10"/>
+      <c r="D35" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1201,39 +1252,11 @@
     <hyperlink ref="G13" r:id="rId12" xr:uid="{1FD6EE7D-6127-482F-A30C-D19E414C6A22}"/>
     <hyperlink ref="G7" r:id="rId13" xr:uid="{B74D72ED-DD1C-4B45-BDC3-95E7563249D4}"/>
     <hyperlink ref="G8" r:id="rId14" xr:uid="{40A6079E-1ED0-4123-8C49-87102BDDFC9B}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{530FF82B-B79C-4F00-9823-E2DE127F6F20}"/>
+    <hyperlink ref="G6" r:id="rId16" xr:uid="{8FBD6C64-0FCA-4CA1-BD0B-CC138746ACBF}"/>
+    <hyperlink ref="G10" r:id="rId17" xr:uid="{16335B64-D26B-48C8-A020-9AE490110F15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19EA82D-1FD1-40C6-BF27-93EEB33B31EF}">
-  <dimension ref="B1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B2" s="1">
-        <f>SUM(D:D)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>